<commit_message>
Some further steps for data cleaning.
</commit_message>
<xml_diff>
--- a/src/original_data/var_info.xlsx
+++ b/src/original_data/var_info.xlsx
@@ -5,17 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berfinbinzet/Desktop/EPP_Project/project/Final_Project/src/original_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berfinbinzet/Desktop/EPP_Project/project/Final_Project/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42614591-A10C-B74A-8B74-1720BFF71643}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7983EB-41D7-B24C-8543-146D875FF56D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="600" windowWidth="26340" windowHeight="14080" xr2:uid="{3D1ABEF0-DFAA-F34E-8AFF-D9F108717ACA}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$130</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="150">
   <si>
     <t>R0215700</t>
   </si>
@@ -210,252 +213,60 @@
     <t>ESR_KEY</t>
   </si>
   <si>
-    <t>R0214901</t>
-  </si>
-  <si>
-    <t>ESR_COL</t>
-  </si>
-  <si>
     <t>R0406300</t>
   </si>
   <si>
-    <t>R0406301</t>
-  </si>
-  <si>
     <t>R0618800</t>
   </si>
   <si>
-    <t>R0618801</t>
-  </si>
-  <si>
     <t>R0898500</t>
   </si>
   <si>
-    <t>R0898501</t>
-  </si>
-  <si>
     <t>R1144700</t>
   </si>
   <si>
-    <t>R1144701</t>
-  </si>
-  <si>
     <t>R1519900</t>
   </si>
   <si>
-    <t>R1519901</t>
-  </si>
-  <si>
     <t>R1890600</t>
   </si>
   <si>
-    <t>R1890601</t>
-  </si>
-  <si>
     <t>R2257700</t>
   </si>
   <si>
-    <t>R2257701</t>
-  </si>
-  <si>
     <t>R2445100</t>
   </si>
   <si>
-    <t>R2445101</t>
-  </si>
-  <si>
     <t>R2870600</t>
   </si>
   <si>
-    <t>R2870700</t>
-  </si>
-  <si>
     <t>R3074300</t>
   </si>
   <si>
-    <t>R3074400</t>
-  </si>
-  <si>
     <t>R3401000</t>
   </si>
   <si>
-    <t>R3401100</t>
-  </si>
-  <si>
     <t>R3656400</t>
   </si>
   <si>
-    <t>R3656500</t>
-  </si>
-  <si>
     <t>R4006900</t>
   </si>
   <si>
-    <t>R4007000</t>
-  </si>
-  <si>
     <t>R4418000</t>
   </si>
   <si>
-    <t>R4418100</t>
-  </si>
-  <si>
     <t>R5081000</t>
   </si>
   <si>
-    <t>R5081100</t>
-  </si>
-  <si>
     <t>R5166300</t>
   </si>
   <si>
-    <t>R5166400</t>
-  </si>
-  <si>
     <t>R6478900</t>
   </si>
   <si>
-    <t>R6479000</t>
-  </si>
-  <si>
     <t>T0988100</t>
   </si>
   <si>
-    <t>T0988200</t>
-  </si>
-  <si>
-    <t>R9900002</t>
-  </si>
-  <si>
-    <t>C1DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 1ST CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9900802</t>
-  </si>
-  <si>
-    <t>C2DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 2ND CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9901602</t>
-  </si>
-  <si>
-    <t>C3DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 3RD CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9902402</t>
-  </si>
-  <si>
-    <t>C4DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 4TH CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9903202</t>
-  </si>
-  <si>
-    <t>C5DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 5TH CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9904002</t>
-  </si>
-  <si>
-    <t>C6DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 6TH CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9904802</t>
-  </si>
-  <si>
-    <t>C7DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 7TH CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9905602</t>
-  </si>
-  <si>
-    <t>C8DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 8TH CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9906202</t>
-  </si>
-  <si>
-    <t>C9DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 9TH CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9906802</t>
-  </si>
-  <si>
-    <t>C10DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 10TH CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R9907402</t>
-  </si>
-  <si>
-    <t>C11DOB~Y</t>
-  </si>
-  <si>
-    <t>DATE OF BIRTH OF 11TH CHILD - YEAR</t>
-  </si>
-  <si>
-    <t>R0000149</t>
-  </si>
-  <si>
-    <t>HHID</t>
-  </si>
-  <si>
-    <t>HOUSEHOLD IDENTIFICATION NUMBER</t>
-  </si>
-  <si>
-    <t>R0174800</t>
-  </si>
-  <si>
-    <t>HHI_FINAL_GENCODE.01</t>
-  </si>
-  <si>
-    <t>R0175700</t>
-  </si>
-  <si>
-    <t>HHI_FINAL_GENCODE.02</t>
-  </si>
-  <si>
-    <t>R0175000</t>
-  </si>
-  <si>
-    <t>HHI_FINAL_AGE.01</t>
-  </si>
-  <si>
-    <t>R0175900</t>
-  </si>
-  <si>
-    <t>HHI_FINAL_AGE.02</t>
-  </si>
-  <si>
     <t>nlsy_name</t>
   </si>
   <si>
@@ -468,25 +279,214 @@
     <t>survey_year</t>
   </si>
   <si>
-    <t>NUMBER OF WEEKS WORKED</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NUMBER OF HOURS WORKED </t>
-  </si>
-  <si>
-    <t>EMPLOYMENT STATUS</t>
-  </si>
-  <si>
-    <t>MALE</t>
-  </si>
-  <si>
-    <t>FEMALE</t>
-  </si>
-  <si>
-    <t>MALE_AGE</t>
-  </si>
-  <si>
-    <t>FEMALE_AGE</t>
+    <t>R0000100</t>
+  </si>
+  <si>
+    <t>CASEID</t>
+  </si>
+  <si>
+    <t>R0169100</t>
+  </si>
+  <si>
+    <t>INCOME-24</t>
+  </si>
+  <si>
+    <t>R0214800</t>
+  </si>
+  <si>
+    <t>SAMPLE_SEX</t>
+  </si>
+  <si>
+    <t>R0216500</t>
+  </si>
+  <si>
+    <t>AGEATINT</t>
+  </si>
+  <si>
+    <t>R0328000</t>
+  </si>
+  <si>
+    <t>R0498500</t>
+  </si>
+  <si>
+    <t>R0782101</t>
+  </si>
+  <si>
+    <t>Q13-5_TRUNC_REVISED</t>
+  </si>
+  <si>
+    <t>R1024001</t>
+  </si>
+  <si>
+    <t>R1410701</t>
+  </si>
+  <si>
+    <t>R1778501</t>
+  </si>
+  <si>
+    <t>R2141601</t>
+  </si>
+  <si>
+    <t>R2350301</t>
+  </si>
+  <si>
+    <t>R2722501</t>
+  </si>
+  <si>
+    <t>R2971401</t>
+  </si>
+  <si>
+    <t>R3279401</t>
+  </si>
+  <si>
+    <t>R3559001</t>
+  </si>
+  <si>
+    <t>R3897101</t>
+  </si>
+  <si>
+    <t>R4295101</t>
+  </si>
+  <si>
+    <t>R4982801</t>
+  </si>
+  <si>
+    <t>R5626201</t>
+  </si>
+  <si>
+    <t>R6364601</t>
+  </si>
+  <si>
+    <t>R6909701</t>
+  </si>
+  <si>
+    <t>R7607800</t>
+  </si>
+  <si>
+    <t>Q13-5_TRUNC</t>
+  </si>
+  <si>
+    <t>R8316300</t>
+  </si>
+  <si>
+    <t>T0912400</t>
+  </si>
+  <si>
+    <t>T2076700</t>
+  </si>
+  <si>
+    <t>T3045300</t>
+  </si>
+  <si>
+    <t>T3977400</t>
+  </si>
+  <si>
+    <t>T4915800</t>
+  </si>
+  <si>
+    <t>T5619500</t>
+  </si>
+  <si>
+    <t>R0406510</t>
+  </si>
+  <si>
+    <t>R0619010</t>
+  </si>
+  <si>
+    <t>R0898310</t>
+  </si>
+  <si>
+    <t>R1145110</t>
+  </si>
+  <si>
+    <t>R1520310</t>
+  </si>
+  <si>
+    <t>R1891010</t>
+  </si>
+  <si>
+    <t>R2258110</t>
+  </si>
+  <si>
+    <t>R2445510</t>
+  </si>
+  <si>
+    <t>R2871300</t>
+  </si>
+  <si>
+    <t>R3075000</t>
+  </si>
+  <si>
+    <t>R3401700</t>
+  </si>
+  <si>
+    <t>R3657100</t>
+  </si>
+  <si>
+    <t>R4007600</t>
+  </si>
+  <si>
+    <t>R4418700</t>
+  </si>
+  <si>
+    <t>R5081700</t>
+  </si>
+  <si>
+    <t>R5167000</t>
+  </si>
+  <si>
+    <t>R6479800</t>
+  </si>
+  <si>
+    <t>R7007500</t>
+  </si>
+  <si>
+    <t>R7704800</t>
+  </si>
+  <si>
+    <t>R8497200</t>
+  </si>
+  <si>
+    <t>T0989000</t>
+  </si>
+  <si>
+    <t>T2210800</t>
+  </si>
+  <si>
+    <t>T3108700</t>
+  </si>
+  <si>
+    <t>T4113200</t>
+  </si>
+  <si>
+    <t>T5023600</t>
+  </si>
+  <si>
+    <t>T5771500</t>
+  </si>
+  <si>
+    <t>hours_worked</t>
+  </si>
+  <si>
+    <t>earnings</t>
+  </si>
+  <si>
+    <t>sex</t>
+  </si>
+  <si>
+    <t>employment_status</t>
+  </si>
+  <si>
+    <t>weeks_worked</t>
+  </si>
+  <si>
+    <t>individual_id</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>invariant</t>
   </si>
 </sst>
 </file>
@@ -855,416 +855,416 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295AFC39-E4A9-E84C-941B-126441E9E3E7}">
-  <dimension ref="A1:D109"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88ECB0D-008C-0041-B40C-8251D6DFE406}">
+  <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="E103" sqref="E103"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="73.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="113" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>140</v>
+        <v>76</v>
       </c>
       <c r="B1" t="s">
-        <v>141</v>
+        <v>77</v>
       </c>
       <c r="C1" t="s">
-        <v>142</v>
+        <v>78</v>
       </c>
       <c r="D1" t="s">
-        <v>143</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>140</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D2" s="1">
-        <v>1979</v>
+        <v>2014</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>2</v>
+        <v>141</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D3" s="1">
-        <v>1980</v>
+        <v>2016</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>3</v>
+        <v>86</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D4" s="1">
-        <v>1981</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>4</v>
+        <v>116</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D5" s="1">
-        <v>1982</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>5</v>
+        <v>117</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D6" s="1">
-        <v>1983</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D7" s="1">
-        <v>1984</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D8" s="1">
-        <v>1985</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
-        <v>8</v>
+        <v>120</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D9" s="1">
-        <v>1986</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>9</v>
+        <v>121</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D10" s="1">
-        <v>1987</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>122</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D11" s="1">
-        <v>1988</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D12" s="1">
-        <v>1989</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
-        <v>12</v>
+        <v>124</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D13" s="1">
-        <v>1990</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>125</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D14" s="1">
-        <v>1991</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>14</v>
+        <v>126</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D15" s="1">
-        <v>1992</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>15</v>
+        <v>127</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D16" s="1">
-        <v>1993</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>16</v>
+        <v>128</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D17" s="1">
-        <v>1994</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>17</v>
+        <v>129</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D18" s="1">
-        <v>1996</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>18</v>
+        <v>130</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D19" s="1">
-        <v>1998</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>19</v>
+        <v>131</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D20" s="1">
-        <v>2000</v>
+        <v>1996</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>20</v>
+        <v>132</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D21" s="1">
-        <v>2002</v>
+        <v>1998</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>21</v>
+        <v>133</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D22" s="1">
-        <v>2004</v>
+        <v>2000</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>22</v>
+        <v>134</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D23" s="1">
-        <v>2006</v>
+        <v>2002</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>23</v>
+        <v>135</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D24" s="1">
-        <v>2008</v>
+        <v>2004</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D25" s="1">
-        <v>2010</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D26" s="1">
-        <v>2012</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>26</v>
+        <v>138</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D27" s="1">
-        <v>2014</v>
+        <v>2010</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>139</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
       <c r="D28" s="1">
-        <v>2016</v>
+        <v>2012</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>28</v>
+        <v>56</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C29" s="1" t="s">
         <v>145</v>
@@ -1275,10 +1275,10 @@
     </row>
     <row r="30" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>30</v>
+        <v>58</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C30" s="1" t="s">
         <v>145</v>
@@ -1289,10 +1289,10 @@
     </row>
     <row r="31" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>145</v>
@@ -1303,10 +1303,10 @@
     </row>
     <row r="32" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>145</v>
@@ -1317,10 +1317,10 @@
     </row>
     <row r="33" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>145</v>
@@ -1331,10 +1331,10 @@
     </row>
     <row r="34" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>62</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C34" s="1" t="s">
         <v>145</v>
@@ -1345,10 +1345,10 @@
     </row>
     <row r="35" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>35</v>
+        <v>63</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>145</v>
@@ -1359,10 +1359,10 @@
     </row>
     <row r="36" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
         <v>145</v>
@@ -1373,10 +1373,10 @@
     </row>
     <row r="37" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
-        <v>37</v>
+        <v>65</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>145</v>
@@ -1387,10 +1387,10 @@
     </row>
     <row r="38" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>38</v>
+        <v>66</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C38" s="1" t="s">
         <v>145</v>
@@ -1401,10 +1401,10 @@
     </row>
     <row r="39" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>39</v>
+        <v>67</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C39" s="1" t="s">
         <v>145</v>
@@ -1415,10 +1415,10 @@
     </row>
     <row r="40" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>40</v>
+        <v>68</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C40" s="1" t="s">
         <v>145</v>
@@ -1429,10 +1429,10 @@
     </row>
     <row r="41" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A41" s="2" t="s">
-        <v>41</v>
+        <v>69</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>145</v>
@@ -1443,10 +1443,10 @@
     </row>
     <row r="42" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>145</v>
@@ -1457,10 +1457,10 @@
     </row>
     <row r="43" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>145</v>
@@ -1471,10 +1471,10 @@
     </row>
     <row r="44" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>145</v>
@@ -1485,10 +1485,10 @@
     </row>
     <row r="45" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
-        <v>45</v>
+        <v>73</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>145</v>
@@ -1499,10 +1499,10 @@
     </row>
     <row r="46" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>46</v>
+        <v>74</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>145</v>
@@ -1513,1072 +1513,1445 @@
     </row>
     <row r="47" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>47</v>
+        <v>75</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>145</v>
       </c>
       <c r="D47" s="1">
-        <v>2000</v>
+        <v>2006</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>48</v>
+        <v>80</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D48" s="1">
-        <v>2002</v>
+        <v>147</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
-        <v>49</v>
+        <v>28</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D49" s="1">
-        <v>2004</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A50" s="2" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D50" s="1">
-        <v>2006</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D51" s="1">
-        <v>2008</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D52" s="1">
-        <v>2010</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D53" s="1">
-        <v>2012</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D54" s="1">
-        <v>2014</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="55" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>29</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="D55" s="1">
-        <v>2016</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="56" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D56" s="1">
-        <v>1979</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D57" s="1">
-        <v>1979</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D58" s="1">
-        <v>1980</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="59" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D59" s="1">
-        <v>1980</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D60" s="1">
-        <v>1981</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D61" s="1">
-        <v>1981</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D62" s="1">
-        <v>1982</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D63" s="1">
-        <v>1982</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D64" s="1">
-        <v>1983</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D65" s="1">
-        <v>1983</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D66" s="1">
-        <v>1984</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D67" s="1">
-        <v>1984</v>
+        <v>1999</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D68" s="1">
-        <v>1985</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D69" s="1">
-        <v>1985</v>
+        <v>2003</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D70" s="1">
-        <v>1986</v>
+        <v>2005</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D71" s="1">
-        <v>1986</v>
+        <v>2007</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D72" s="1">
-        <v>1987</v>
+        <v>2009</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A73" s="2" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D73" s="1">
-        <v>1987</v>
+        <v>2011</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D74" s="1">
-        <v>1988</v>
+        <v>2013</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>59</v>
+        <v>29</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D75" s="1">
-        <v>1988</v>
+        <v>2015</v>
       </c>
     </row>
     <row r="76" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>78</v>
+        <v>0</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D76" s="1">
-        <v>1989</v>
+        <v>1978</v>
       </c>
     </row>
     <row r="77" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
-        <v>79</v>
+        <v>2</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D77" s="1">
-        <v>1989</v>
+        <v>1979</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>80</v>
+        <v>3</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D78" s="1">
-        <v>1990</v>
+        <v>1980</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>81</v>
+        <v>4</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D79" s="1">
-        <v>1990</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>82</v>
+        <v>5</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D80" s="1">
-        <v>1991</v>
+        <v>1982</v>
       </c>
     </row>
     <row r="81" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
-        <v>83</v>
+        <v>6</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D81" s="1">
-        <v>1991</v>
+        <v>1983</v>
       </c>
     </row>
     <row r="82" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D82" s="1">
-        <v>1992</v>
+        <v>1984</v>
       </c>
     </row>
     <row r="83" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D83" s="1">
-        <v>1992</v>
+        <v>1985</v>
       </c>
     </row>
     <row r="84" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>86</v>
+        <v>9</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D84" s="1">
-        <v>1993</v>
+        <v>1986</v>
       </c>
     </row>
     <row r="85" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A85" s="2" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D85" s="1">
-        <v>1993</v>
+        <v>1987</v>
       </c>
     </row>
     <row r="86" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>88</v>
+        <v>11</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D86" s="1">
-        <v>1994</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="87" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>89</v>
+        <v>12</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D87" s="1">
-        <v>1994</v>
+        <v>1989</v>
       </c>
     </row>
     <row r="88" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>90</v>
+        <v>13</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D88" s="1">
-        <v>1996</v>
+        <v>1990</v>
       </c>
     </row>
     <row r="89" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A89" s="2" t="s">
-        <v>91</v>
+        <v>14</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D89" s="1">
-        <v>1996</v>
+        <v>1991</v>
       </c>
     </row>
     <row r="90" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>92</v>
+        <v>15</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D90" s="1">
-        <v>1998</v>
+        <v>1992</v>
       </c>
     </row>
     <row r="91" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>93</v>
+        <v>16</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D91" s="1">
-        <v>1998</v>
+        <v>1993</v>
       </c>
     </row>
     <row r="92" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>94</v>
+        <v>17</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>57</v>
+        <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D92" s="1">
-        <v>2006</v>
+        <v>1995</v>
       </c>
     </row>
     <row r="93" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A93" s="2" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>59</v>
+        <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>146</v>
       </c>
       <c r="D93" s="1">
-        <v>2006</v>
+        <v>1997</v>
       </c>
     </row>
     <row r="94" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>96</v>
+        <v>19</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>97</v>
+        <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="D94" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="D94" s="1">
+        <v>1999</v>
+      </c>
     </row>
     <row r="95" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A95" s="2" t="s">
-        <v>99</v>
+        <v>20</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>100</v>
+        <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="D95" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="D95" s="1">
+        <v>2001</v>
+      </c>
     </row>
     <row r="96" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A96" s="2" t="s">
-        <v>102</v>
+        <v>21</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>103</v>
+        <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D96" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="D96" s="1">
+        <v>2003</v>
+      </c>
     </row>
     <row r="97" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A97" s="2" t="s">
-        <v>105</v>
+        <v>22</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>106</v>
+        <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="D97" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="D97" s="1">
+        <v>2005</v>
+      </c>
     </row>
     <row r="98" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>108</v>
+        <v>23</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>109</v>
+        <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="D98" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="D98" s="1">
+        <v>2007</v>
+      </c>
     </row>
     <row r="99" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>111</v>
+        <v>24</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>112</v>
+        <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="D99" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="D99" s="1">
+        <v>2009</v>
+      </c>
     </row>
     <row r="100" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A100" s="2" t="s">
-        <v>114</v>
+        <v>25</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D100" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="D100" s="1">
+        <v>2011</v>
+      </c>
     </row>
     <row r="101" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A101" s="2" t="s">
-        <v>117</v>
+        <v>26</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>118</v>
+        <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>119</v>
-      </c>
-      <c r="D101" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="D101" s="1">
+        <v>2013</v>
+      </c>
     </row>
     <row r="102" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A102" s="2" t="s">
-        <v>120</v>
+        <v>27</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>121</v>
+        <v>1</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D102" s="1"/>
+        <v>146</v>
+      </c>
+      <c r="D102" s="1">
+        <v>2015</v>
+      </c>
     </row>
     <row r="103" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A103" s="2" t="s">
-        <v>123</v>
+        <v>84</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>124</v>
+        <v>85</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D103" s="1"/>
+        <v>144</v>
+      </c>
+      <c r="D103" s="1" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="104" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>126</v>
+        <v>82</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>127</v>
+        <v>83</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="D104" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="D104" s="1">
+        <v>1978</v>
+      </c>
     </row>
     <row r="105" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>130</v>
+        <v>83</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D105" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="D105" s="1">
+        <v>1979</v>
+      </c>
     </row>
     <row r="106" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>133</v>
+        <v>83</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D106" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="D106" s="1">
+        <v>1980</v>
+      </c>
     </row>
     <row r="107" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A107" s="2" t="s">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D107" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="D107" s="1">
+        <v>2001</v>
+      </c>
     </row>
     <row r="108" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A108" s="2" t="s">
-        <v>136</v>
+        <v>109</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>137</v>
+        <v>108</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D108" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="D108" s="1">
+        <v>2003</v>
+      </c>
     </row>
     <row r="109" spans="1:4" ht="18" x14ac:dyDescent="0.2">
       <c r="A109" s="2" t="s">
-        <v>138</v>
+        <v>110</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>139</v>
+        <v>108</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D109" s="1"/>
+        <v>143</v>
+      </c>
+      <c r="D109" s="1">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A110" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B110" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D110" s="1">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A111" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="B111" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D111" s="1">
+        <v>2013</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A112" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="B112" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D112" s="1">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A113" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B113" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D113" s="1">
+        <v>1981</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A114" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="B114" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D114" s="1">
+        <v>1982</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A115" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B115" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D115" s="1">
+        <v>1983</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A116" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B116" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C116" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D116" s="1">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A117" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B117" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C117" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D117" s="1">
+        <v>1985</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A118" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="B118" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D118" s="1">
+        <v>1986</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A119" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B119" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D119" s="1">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="120" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A120" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B120" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D120" s="1">
+        <v>1988</v>
+      </c>
+    </row>
+    <row r="121" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A121" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B121" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D121" s="1">
+        <v>1989</v>
+      </c>
+    </row>
+    <row r="122" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A122" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B122" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D122" s="1">
+        <v>1990</v>
+      </c>
+    </row>
+    <row r="123" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A123" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B123" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D123" s="1">
+        <v>1991</v>
+      </c>
+    </row>
+    <row r="124" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A124" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="B124" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C124" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D124" s="1">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="125" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A125" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B125" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D125" s="1">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="126" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A126" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="B126" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C126" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D126" s="1">
+        <v>1997</v>
+      </c>
+    </row>
+    <row r="127" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A127" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B127" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C127" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D127" s="1">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A128" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B128" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C128" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D128" s="1">
+        <v>2007</v>
+      </c>
+    </row>
+    <row r="129" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A129" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C129" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D129" s="1">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="130" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+      <c r="A130" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="B130" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C130" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D130" s="1">
+        <v>1992</v>
+      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:D130" xr:uid="{68889205-04C2-0E47-A671-2DD8C58C36FC}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D130">
+      <sortCondition ref="C1:C130"/>
+    </sortState>
+  </autoFilter>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0BBB9833-B57D-1645-9C74-A982990A5D37}"/>
-    <hyperlink ref="B2" r:id="rId2" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C82A8DDD-E2A7-BC40-AE27-6D026DFBF143}"/>
-    <hyperlink ref="A3" r:id="rId3" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F9A8AC80-680C-024F-9FAC-ACF2CBCB8616}"/>
-    <hyperlink ref="B3" r:id="rId4" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AF144475-A962-6A41-9822-7DC805793713}"/>
-    <hyperlink ref="A4" r:id="rId5" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{ED7DA822-CF18-6645-ABBA-FF2BB098BEF3}"/>
-    <hyperlink ref="B4" r:id="rId6" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{78DC5AFC-9D64-CA4C-B2E7-B8FC545E9833}"/>
-    <hyperlink ref="A5" r:id="rId7" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{68F5BECA-7DEF-C147-9485-7449E32ADACE}"/>
-    <hyperlink ref="B5" r:id="rId8" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4E6D682D-D907-A34A-B397-3412F9AE086B}"/>
-    <hyperlink ref="A6" r:id="rId9" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A7C08A21-A383-B041-9E0C-3F680E9E0CF7}"/>
-    <hyperlink ref="B6" r:id="rId10" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C1E48C75-135F-9F4E-9F49-053AA2FDC467}"/>
-    <hyperlink ref="A7" r:id="rId11" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{866CCE02-B7C9-8849-ADCB-DAAC29183E6B}"/>
-    <hyperlink ref="B7" r:id="rId12" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B75AC787-B361-EF4E-A410-15E6B82C3113}"/>
-    <hyperlink ref="A8" r:id="rId13" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1028FCBE-793B-B544-9B62-2955F07B5919}"/>
-    <hyperlink ref="B8" r:id="rId14" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{68598F7B-AF7B-F54C-A99E-2A0557061D4F}"/>
-    <hyperlink ref="A9" r:id="rId15" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{613F1056-6F8A-404D-A89D-5342B22B593F}"/>
-    <hyperlink ref="B9" r:id="rId16" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A53C6BE0-AC44-8842-B384-97BD16E63FCC}"/>
-    <hyperlink ref="A10" r:id="rId17" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FBC18480-9BB6-F942-A154-96DC349A1FE1}"/>
-    <hyperlink ref="B10" r:id="rId18" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{62638396-23B7-6543-8186-38F3D9044259}"/>
-    <hyperlink ref="A11" r:id="rId19" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4CD3F7D5-D29B-454B-964D-1F0EA197E9D5}"/>
-    <hyperlink ref="B11" r:id="rId20" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B751F1E4-C3A9-3246-810F-8D26A6C02ED9}"/>
-    <hyperlink ref="A12" r:id="rId21" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5194A9A8-8A80-F24B-8F2C-857A2FB97ACA}"/>
-    <hyperlink ref="B12" r:id="rId22" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{74B9B7CE-7482-E543-9455-38C717C9E679}"/>
-    <hyperlink ref="A13" r:id="rId23" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{70BB856E-A1E8-6847-AC73-C7F0B006E89C}"/>
-    <hyperlink ref="B13" r:id="rId24" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1BD025F4-A88F-6B42-8363-276196599D1B}"/>
-    <hyperlink ref="A14" r:id="rId25" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E0545D30-9E67-6E47-988D-E2309F4E6F1A}"/>
-    <hyperlink ref="B14" r:id="rId26" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1D2763DE-9988-E841-B686-35AD81A399D5}"/>
-    <hyperlink ref="A15" r:id="rId27" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F1445E26-BD22-F942-884A-CE8EA69FDC25}"/>
-    <hyperlink ref="B15" r:id="rId28" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C7DD52DC-AF50-C840-8E55-A7E90BD23105}"/>
-    <hyperlink ref="A16" r:id="rId29" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F0DC388E-6A64-954A-BF96-BF6A176E74D4}"/>
-    <hyperlink ref="B16" r:id="rId30" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2971ACFF-E7CF-0D4C-92B8-C4729694E55D}"/>
-    <hyperlink ref="A17" r:id="rId31" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2B2D31CD-025A-3345-A373-C787C24C0FF0}"/>
-    <hyperlink ref="B17" r:id="rId32" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B96994C2-4D6B-7244-A224-18478CD89B25}"/>
-    <hyperlink ref="A18" r:id="rId33" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2C8BA924-E488-F149-8A57-3B22D08C0E8E}"/>
-    <hyperlink ref="B18" r:id="rId34" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0505AE05-1F4E-7842-8C79-BB7CE9B35EFB}"/>
-    <hyperlink ref="A19" r:id="rId35" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{86310658-81AE-9343-AE17-480F21918687}"/>
-    <hyperlink ref="B19" r:id="rId36" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{589B1378-B4AF-0144-91E4-A1C8D1F65153}"/>
-    <hyperlink ref="A20" r:id="rId37" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7377BA2A-C80A-CD4C-B476-80748D62363E}"/>
-    <hyperlink ref="B20" r:id="rId38" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{24DB127A-E685-7F4F-86DE-B0055049CD57}"/>
-    <hyperlink ref="A21" r:id="rId39" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{97EE7882-9A80-3E49-976B-82D30C1D7ED2}"/>
-    <hyperlink ref="B21" r:id="rId40" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{057413EF-63BD-704E-996A-0E46FE9D655E}"/>
-    <hyperlink ref="A22" r:id="rId41" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{83090A7D-34C4-A84C-B083-673FA9554782}"/>
-    <hyperlink ref="B22" r:id="rId42" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4E42AC9C-9CFC-B747-97A5-E868DDE6A234}"/>
-    <hyperlink ref="A23" r:id="rId43" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{DF206652-2648-0B4A-9166-454B23B358C2}"/>
-    <hyperlink ref="B23" r:id="rId44" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{701BCDBC-326E-1A4C-BBAC-FCAB9FFD488C}"/>
-    <hyperlink ref="A24" r:id="rId45" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AC29F00E-1907-A443-BDB1-52ADDC19794D}"/>
-    <hyperlink ref="B24" r:id="rId46" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1AC5B4A0-E4C3-1741-A8FD-C38A348C40DD}"/>
-    <hyperlink ref="A25" r:id="rId47" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CA44A335-B909-244F-B3F9-A00BBE96925A}"/>
-    <hyperlink ref="B25" r:id="rId48" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8FEC60AB-FABE-3448-9126-165810ADF803}"/>
-    <hyperlink ref="A26" r:id="rId49" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{40020342-8307-E943-A828-4E0FB964D9E9}"/>
-    <hyperlink ref="B26" r:id="rId50" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{479DD46B-F140-9A4E-A342-B9EBC74FE56F}"/>
-    <hyperlink ref="A27" r:id="rId51" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0CDD391F-9B85-DC4A-ADC6-F6710E18097E}"/>
-    <hyperlink ref="B27" r:id="rId52" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2BE4B2B0-76DB-8249-8843-CADAFCDAF288}"/>
-    <hyperlink ref="A28" r:id="rId53" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9CA88BEA-825A-5D4B-984F-A92BBFFE09F0}"/>
-    <hyperlink ref="B28" r:id="rId54" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{697F42F5-DA7C-9347-A070-C67AF9DB00FF}"/>
-    <hyperlink ref="A29" r:id="rId55" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3D843971-BF30-BA4C-B54D-BD8686A5FE58}"/>
-    <hyperlink ref="B29" r:id="rId56" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1EA726D5-3F27-1B4B-A731-5F1F480809FA}"/>
-    <hyperlink ref="A30" r:id="rId57" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E90B168A-272A-6948-93A1-0BC1E486D397}"/>
-    <hyperlink ref="B30" r:id="rId58" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3DE24DB1-ABFF-D542-9515-6B229E5E2E08}"/>
-    <hyperlink ref="A31" r:id="rId59" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5947F91B-F569-D049-9476-5AA6C0E643D1}"/>
-    <hyperlink ref="B31" r:id="rId60" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C56AF7AE-D13D-7542-91DB-587C29A7AEA7}"/>
-    <hyperlink ref="A32" r:id="rId61" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AC2B7CB4-CAA9-9447-9ABF-EF995048085A}"/>
-    <hyperlink ref="B32" r:id="rId62" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{88FD4E48-7CE0-E043-9A9F-02487DE7DADC}"/>
-    <hyperlink ref="A33" r:id="rId63" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D833953F-2E92-0342-BF92-751E1FCCE996}"/>
-    <hyperlink ref="B33" r:id="rId64" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FBB044DD-3F38-864C-B0B0-4C7B3CEB34B2}"/>
-    <hyperlink ref="A34" r:id="rId65" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D842F6F8-BC5E-404E-9B8B-3F2CD88F172A}"/>
-    <hyperlink ref="B34" r:id="rId66" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{524DFB31-6BCD-E14E-9C42-119F319B577A}"/>
-    <hyperlink ref="A35" r:id="rId67" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FAF52936-2B39-E24E-A8F1-CED83C0B22FD}"/>
-    <hyperlink ref="B35" r:id="rId68" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D830D659-F2C9-7E4E-B5D7-A223EAD21354}"/>
-    <hyperlink ref="A36" r:id="rId69" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{981FF50D-BF7B-2E49-856B-B3D1D6DAF74A}"/>
-    <hyperlink ref="B36" r:id="rId70" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7C1752B7-B66D-F246-A35D-D7A0BF89BF18}"/>
-    <hyperlink ref="A37" r:id="rId71" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6C2006DA-0DC4-EE49-8341-28278FFE3B34}"/>
-    <hyperlink ref="B37" r:id="rId72" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1A0847E3-83BC-F243-B6B2-C8E9B4469226}"/>
-    <hyperlink ref="A38" r:id="rId73" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{90444957-B9CF-3845-9C87-146BBB6D812D}"/>
-    <hyperlink ref="B38" r:id="rId74" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FFD2520E-EDDD-C442-AF43-E0171AFE11E9}"/>
-    <hyperlink ref="A39" r:id="rId75" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{58607837-EB9D-D548-B05D-F0E081773247}"/>
-    <hyperlink ref="B39" r:id="rId76" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{086EF71A-B22A-8941-9A06-0FC10B08CB7F}"/>
-    <hyperlink ref="A40" r:id="rId77" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3F362F76-792A-F341-9C78-280A166F9E70}"/>
-    <hyperlink ref="B40" r:id="rId78" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{662F532B-D069-974C-B691-842921027C2B}"/>
-    <hyperlink ref="A41" r:id="rId79" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F021433D-E8C9-8744-B1E2-77E8D138D8C4}"/>
-    <hyperlink ref="B41" r:id="rId80" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{38CB1B2E-CD2F-6C42-8C79-8AF3EAC1A374}"/>
-    <hyperlink ref="A42" r:id="rId81" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5CDA93CD-18A8-EE45-9338-E398A3AA9536}"/>
-    <hyperlink ref="B42" r:id="rId82" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CD8689F6-2B51-854F-8072-9D163546F801}"/>
-    <hyperlink ref="A43" r:id="rId83" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9E2AC834-93A8-3B41-90C1-1343FA1AD18C}"/>
-    <hyperlink ref="B43" r:id="rId84" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CE3188FD-35D1-E441-9842-44B4D35AC2B4}"/>
-    <hyperlink ref="A44" r:id="rId85" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CD0BD377-1865-2C40-94D7-69FBC1E4CDA7}"/>
-    <hyperlink ref="B44" r:id="rId86" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E6A98D3B-70AF-F246-A2A1-E952A0EF5EEE}"/>
-    <hyperlink ref="A45" r:id="rId87" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{958DDEED-0E77-3F45-B465-8D52FACCD91C}"/>
-    <hyperlink ref="B45" r:id="rId88" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3FF758D6-F198-B64F-A7E2-0EE9DF23A662}"/>
-    <hyperlink ref="A46" r:id="rId89" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B9415841-3AC6-754C-B9BB-F8CE8C57E1AB}"/>
-    <hyperlink ref="B46" r:id="rId90" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BA834863-2A7D-D640-953F-983032750074}"/>
-    <hyperlink ref="A47" r:id="rId91" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C260D099-E4A1-BF43-B443-1C3F4F3E343E}"/>
-    <hyperlink ref="B47" r:id="rId92" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AC6EE9CE-04BB-464B-8ECA-7AF42A43F698}"/>
-    <hyperlink ref="A48" r:id="rId93" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C0BC9C7D-1AAE-2042-BBE8-81BF848135F5}"/>
-    <hyperlink ref="B48" r:id="rId94" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{783DE4DB-DE74-E64B-B3CE-473DA390D7C3}"/>
-    <hyperlink ref="A49" r:id="rId95" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0D3A7C5C-40D4-3540-B9DF-2E7D3D8AAAB3}"/>
-    <hyperlink ref="B49" r:id="rId96" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C63DA11B-248A-2747-89F1-CB7B00F8F2EE}"/>
-    <hyperlink ref="A50" r:id="rId97" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0C6E8BA0-0CA4-C949-8219-BDEBB3C117ED}"/>
-    <hyperlink ref="B50" r:id="rId98" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8C4C30B4-75C2-0840-81F1-71ABA6A75236}"/>
-    <hyperlink ref="A51" r:id="rId99" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E023B8FE-E6B1-A449-8D51-DE31F3BCB260}"/>
-    <hyperlink ref="B51" r:id="rId100" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7ABB5A2D-32C3-C44F-8182-46A1A6F434A9}"/>
-    <hyperlink ref="A52" r:id="rId101" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2D33EFB4-B7B1-F043-B715-281A19C74AA2}"/>
-    <hyperlink ref="B52" r:id="rId102" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{505CC6BC-77BD-7A42-8641-32C8238BAA0F}"/>
-    <hyperlink ref="A53" r:id="rId103" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9CBF64B9-2208-CF48-BB78-9006040D63BB}"/>
-    <hyperlink ref="B53" r:id="rId104" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8FCFA000-08F6-F941-9632-53B0DB62E186}"/>
-    <hyperlink ref="A54" r:id="rId105" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1514D463-2306-9A4C-A380-4F0E23B70B7C}"/>
-    <hyperlink ref="B54" r:id="rId106" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D2EDC3CA-8E39-3441-8929-66D9E0273D25}"/>
-    <hyperlink ref="A55" r:id="rId107" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{EB49AF0F-DF32-E248-8B2F-D57FCE998D67}"/>
-    <hyperlink ref="B55" r:id="rId108" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{36898472-A960-8E4A-9296-AA45DDD85471}"/>
-    <hyperlink ref="A56" r:id="rId109" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9810C7F4-85F1-6E4A-986B-BDFA2A4838FA}"/>
-    <hyperlink ref="B56" r:id="rId110" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{15E84502-B737-8C46-A1D3-836D021C75F2}"/>
-    <hyperlink ref="A57" r:id="rId111" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A10C2793-0422-7046-9973-1D36EA5848E5}"/>
-    <hyperlink ref="B57" r:id="rId112" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E9E75E59-5B93-3E45-8B8F-E3F7BA442AA1}"/>
-    <hyperlink ref="A58" r:id="rId113" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{699CAA75-BFFA-9440-8EB7-C9FD3C936BB3}"/>
-    <hyperlink ref="B58" r:id="rId114" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E14CC8A0-6D19-2C4E-A985-FEBDDFA3D85C}"/>
-    <hyperlink ref="A59" r:id="rId115" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{804E7B62-DC8F-CD4A-BAF9-0A4775A5DB41}"/>
-    <hyperlink ref="B59" r:id="rId116" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7C9CA98A-4C02-3D4A-87B6-72C59C5549B9}"/>
-    <hyperlink ref="A60" r:id="rId117" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C8CA672F-AF64-0244-91AF-DED45F63EBB5}"/>
-    <hyperlink ref="B60" r:id="rId118" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{21A1CE3D-E5E0-4B4D-89BB-F2D518513839}"/>
-    <hyperlink ref="A61" r:id="rId119" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F88DD2D2-61A9-CE43-B82F-FD0081D683EF}"/>
-    <hyperlink ref="B61" r:id="rId120" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5DE73578-83AE-5D40-AA05-B742DECE284A}"/>
-    <hyperlink ref="A62" r:id="rId121" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{148DB18A-7ED9-7740-B0B0-7A51ED7918BC}"/>
-    <hyperlink ref="B62" r:id="rId122" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6294FAB7-672F-A948-8E80-803E09A5AAB4}"/>
-    <hyperlink ref="A63" r:id="rId123" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{845D2CEE-2FE1-C143-A2C0-613B4BBE056A}"/>
-    <hyperlink ref="B63" r:id="rId124" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{70CB421D-4C35-FA42-BFBA-21FEDBA2D0F4}"/>
-    <hyperlink ref="A64" r:id="rId125" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9F79D7E0-2554-FD4A-BE35-F51C54F42E8F}"/>
-    <hyperlink ref="B64" r:id="rId126" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0E0ACC5C-770C-134F-B9DF-BECC58191AB1}"/>
-    <hyperlink ref="A65" r:id="rId127" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{745E1A31-E43F-3F48-BBAE-4F98E9608A2E}"/>
-    <hyperlink ref="B65" r:id="rId128" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B4CF7562-CA5F-7C42-B762-091AA7CFC303}"/>
-    <hyperlink ref="A66" r:id="rId129" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{325D0E83-4C0B-E64F-83EF-9FF452F2173C}"/>
-    <hyperlink ref="B66" r:id="rId130" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6E77ACAE-5A0F-1B45-BF8D-A09D963F24EB}"/>
-    <hyperlink ref="A67" r:id="rId131" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A2233292-08C7-A945-8CFE-67390E5FCEA6}"/>
-    <hyperlink ref="B67" r:id="rId132" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C0A8D0F5-8BC7-3B4D-899D-DFDC1FF2361F}"/>
-    <hyperlink ref="A68" r:id="rId133" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{86A2E04C-C76F-B048-B90A-9FA140C4D875}"/>
-    <hyperlink ref="B68" r:id="rId134" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CA211368-79B5-B14B-9499-6649A0521800}"/>
-    <hyperlink ref="A69" r:id="rId135" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{212337B7-2E88-1B4B-8DF0-AAB696B00063}"/>
-    <hyperlink ref="B69" r:id="rId136" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FF589973-FA40-864D-A303-0F16AFA032C2}"/>
-    <hyperlink ref="A70" r:id="rId137" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D372C775-B33D-4742-B92D-760417E8B5F1}"/>
-    <hyperlink ref="B70" r:id="rId138" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CFE19FE3-F0D5-4B43-9965-001293186B05}"/>
-    <hyperlink ref="A71" r:id="rId139" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6EF34C6D-617D-3A4C-9E40-C403C43A4D3E}"/>
-    <hyperlink ref="B71" r:id="rId140" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{584F41F2-78E1-EA4F-A0E0-020B6F9BE57D}"/>
-    <hyperlink ref="A72" r:id="rId141" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5C8BD121-4684-F540-8E70-7AA0B3798BB9}"/>
-    <hyperlink ref="B72" r:id="rId142" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3FD0D76E-E0EF-AD41-B301-965DBFB486BD}"/>
-    <hyperlink ref="A73" r:id="rId143" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5D37453A-812B-D845-8AA7-471740A2104A}"/>
-    <hyperlink ref="B73" r:id="rId144" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F81FFA26-8E11-494D-A4B8-5926E16881BB}"/>
-    <hyperlink ref="A74" r:id="rId145" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8A031551-EC06-5E49-902E-E12C98509FB5}"/>
-    <hyperlink ref="B74" r:id="rId146" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CDE3534F-8C24-E84C-96B1-14D5684D52CD}"/>
-    <hyperlink ref="A75" r:id="rId147" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8171F9B8-A121-5444-B540-DF40199C91BC}"/>
-    <hyperlink ref="B75" r:id="rId148" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2970AE53-D8D0-9843-9414-4F7A4A234A79}"/>
-    <hyperlink ref="A76" r:id="rId149" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{95349186-2991-434C-B75F-57BBE996FDA6}"/>
-    <hyperlink ref="B76" r:id="rId150" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FBE427F4-1C1D-DE45-98D5-641337B0BBBF}"/>
-    <hyperlink ref="A77" r:id="rId151" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7AA06196-1507-C448-9E5B-13147D679EF2}"/>
-    <hyperlink ref="B77" r:id="rId152" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C9135AB0-04BE-4843-8CD9-00F19BF248B4}"/>
-    <hyperlink ref="A78" r:id="rId153" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8C27F961-539C-FF40-B1A8-96B258F53CE4}"/>
-    <hyperlink ref="B78" r:id="rId154" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{751743EB-E94C-4145-A60A-51EC7908DE46}"/>
-    <hyperlink ref="A79" r:id="rId155" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B96A4752-9BC0-6943-B544-0131DBD9820F}"/>
-    <hyperlink ref="B79" r:id="rId156" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{10EB2D0E-F456-B745-A8CE-C97436183B8C}"/>
-    <hyperlink ref="A80" r:id="rId157" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2FAE7660-5311-0345-A67C-0F09E28A4A37}"/>
-    <hyperlink ref="B80" r:id="rId158" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{22F43CF0-F6F4-A745-B570-5CA5B8D2FE86}"/>
-    <hyperlink ref="A81" r:id="rId159" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8DA0D183-8FAB-CA41-94F0-89680B0DEF8E}"/>
-    <hyperlink ref="B81" r:id="rId160" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{384B676D-D604-054B-9413-67918D2D2AF3}"/>
-    <hyperlink ref="A82" r:id="rId161" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{EE31C5D2-3780-6A43-B816-46CE9E1C6D8C}"/>
-    <hyperlink ref="B82" r:id="rId162" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{90A7FDFE-F386-3544-8C7A-0BE147DBEE11}"/>
-    <hyperlink ref="A83" r:id="rId163" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{51C50C10-2AB5-6D41-8BFE-DCF90F4018FB}"/>
-    <hyperlink ref="B83" r:id="rId164" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{841A7836-6015-D244-8B83-3D0212B017A2}"/>
-    <hyperlink ref="A84" r:id="rId165" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2E129E5C-F47E-7545-AD8A-41F3068A4FC4}"/>
-    <hyperlink ref="B84" r:id="rId166" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A6F9F425-648D-B34D-B594-F7087B8ADF72}"/>
-    <hyperlink ref="A85" r:id="rId167" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BD2E8397-8DA0-FF4B-8C14-7C3511208487}"/>
-    <hyperlink ref="B85" r:id="rId168" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{00BD0DD3-EB2C-0345-98F3-96BB4554990D}"/>
-    <hyperlink ref="A86" r:id="rId169" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8A39B713-25AA-FA4B-B622-734F290302F3}"/>
-    <hyperlink ref="B86" r:id="rId170" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4D146487-F454-BC46-9557-C29BFA676064}"/>
-    <hyperlink ref="A87" r:id="rId171" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{079F6746-FEC0-C64D-9546-DCA0A46CDC65}"/>
-    <hyperlink ref="B87" r:id="rId172" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D4C6A362-9280-AB45-AB4B-272721D42C58}"/>
-    <hyperlink ref="A88" r:id="rId173" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{ABC8A246-4C55-8844-9047-18E1C268D74E}"/>
-    <hyperlink ref="B88" r:id="rId174" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{09C06A42-3087-D240-A870-658DC36D335B}"/>
-    <hyperlink ref="A89" r:id="rId175" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{75EA8C69-AB6A-FC42-AE98-9DF8A8E23AF0}"/>
-    <hyperlink ref="B89" r:id="rId176" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{61EB62E1-A0CA-2F43-8FF8-927166D7F35D}"/>
-    <hyperlink ref="A90" r:id="rId177" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7E5CA556-4631-E54B-B0D7-A7B579F16025}"/>
-    <hyperlink ref="B90" r:id="rId178" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E0A92E82-15CF-6A4C-A8FF-5137CAEC4B3C}"/>
-    <hyperlink ref="A91" r:id="rId179" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{61B48091-7C85-C149-A4F1-E4B3BB80C07D}"/>
-    <hyperlink ref="B91" r:id="rId180" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6E2BCC56-E5FC-674B-9688-40C7243696AC}"/>
-    <hyperlink ref="A92" r:id="rId181" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{22EB479D-F127-424F-88BC-33C66B9FB335}"/>
-    <hyperlink ref="B92" r:id="rId182" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FE5073F0-B1AA-2D44-84F5-B0BC2D5A8F18}"/>
-    <hyperlink ref="A93" r:id="rId183" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4B62F710-DBF3-C745-8DA2-E99EA727764A}"/>
-    <hyperlink ref="B93" r:id="rId184" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FEC44981-A5FC-BF43-A946-95A2D6ABF75F}"/>
-    <hyperlink ref="A94" r:id="rId185" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0168641C-40C3-1E45-8B0E-980B68541B28}"/>
-    <hyperlink ref="B94" r:id="rId186" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D06DF123-9055-8C46-8515-18BB5DBDAF35}"/>
-    <hyperlink ref="A95" r:id="rId187" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0E8A8FBE-8C38-FC4E-993E-65BCF6F7A844}"/>
-    <hyperlink ref="B95" r:id="rId188" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{312092CD-36E7-4849-ADFD-E51EDB7A58F4}"/>
-    <hyperlink ref="A96" r:id="rId189" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{60E996F3-8E06-F043-921C-4D22E4F3DF49}"/>
-    <hyperlink ref="B96" r:id="rId190" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AE30D98A-68D1-BD4E-9D73-C6ADF3C5ED1E}"/>
-    <hyperlink ref="A97" r:id="rId191" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A74053F2-9899-3342-9690-6B757AE918AA}"/>
-    <hyperlink ref="B97" r:id="rId192" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3C9ABEBD-1A44-5643-8CDC-AD60B68DE87D}"/>
-    <hyperlink ref="A98" r:id="rId193" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0CBF0B84-D800-B243-BBE0-D0A910AC7BA1}"/>
-    <hyperlink ref="B98" r:id="rId194" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A579F2D8-02F7-4944-B4ED-9454750E2A7B}"/>
-    <hyperlink ref="A99" r:id="rId195" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C1F0CF30-A6D6-C442-B551-CBCBB755AF5E}"/>
-    <hyperlink ref="B99" r:id="rId196" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9C5EDFC5-A59F-6343-9789-6351C5FDA9F2}"/>
-    <hyperlink ref="A100" r:id="rId197" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9AB5303A-F77E-FE43-8648-025869922924}"/>
-    <hyperlink ref="B100" r:id="rId198" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0A8E1CD3-060A-6F4B-905F-09CFC35D140E}"/>
-    <hyperlink ref="A101" r:id="rId199" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4610B86E-541C-CB47-B185-BB450AA6166D}"/>
-    <hyperlink ref="B101" r:id="rId200" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{65C3A21B-E54F-7D4B-9E16-7D69547BD395}"/>
-    <hyperlink ref="A102" r:id="rId201" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{82205E3D-2CEC-F841-A570-3759954BE0BF}"/>
-    <hyperlink ref="B102" r:id="rId202" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0D24F221-D397-2A46-944D-F56E3CD73F07}"/>
-    <hyperlink ref="A103" r:id="rId203" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1E0B0A77-6451-7645-87C9-D7C984F06760}"/>
-    <hyperlink ref="B103" r:id="rId204" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{06BF41AE-C4BF-5444-AA74-C0127E602537}"/>
-    <hyperlink ref="A104" r:id="rId205" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8A772D78-3CA5-094F-8836-35395CAACBE2}"/>
-    <hyperlink ref="B104" r:id="rId206" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2B3C67C1-8FE9-5E47-9D58-09355B875B62}"/>
-    <hyperlink ref="A105" r:id="rId207" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C47A7D8C-E254-A246-9BA4-3C68F954B95F}"/>
-    <hyperlink ref="B105" r:id="rId208" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E7304B98-64D5-0F4E-AC4E-5BF6CB034501}"/>
-    <hyperlink ref="A106" r:id="rId209" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{DBA5840C-9766-9147-85DE-34FD7186E0A9}"/>
-    <hyperlink ref="B106" r:id="rId210" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CD819467-0ED8-1C4B-9137-236675E7899D}"/>
-    <hyperlink ref="A107" r:id="rId211" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{DFD6983D-AE74-864C-99C1-2B2D96ECB667}"/>
-    <hyperlink ref="B107" r:id="rId212" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{90FB3452-2CB5-D349-9F69-80FFC1A0B34B}"/>
-    <hyperlink ref="A108" r:id="rId213" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AFD0DDF0-CCD1-EC4F-B5D9-99EA114E1C9E}"/>
-    <hyperlink ref="B108" r:id="rId214" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FD3ED373-AD9D-3D42-9AB9-779C5C014F35}"/>
-    <hyperlink ref="A109" r:id="rId215" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{73D757C4-0958-B84D-A6D5-78B52BEC7AAF}"/>
-    <hyperlink ref="B109" r:id="rId216" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{10AEA40B-0735-A442-B72F-F5A2D0C04D74}"/>
+    <hyperlink ref="A48" r:id="rId1" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E12BF7E6-8E84-3149-87BE-BB69AB443E3B}"/>
+    <hyperlink ref="B48" r:id="rId2" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{497DC410-400A-DD40-B092-69365819E09D}"/>
+    <hyperlink ref="A104" r:id="rId3" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{DD4C485E-C99C-BB41-BA88-40EA8D316E01}"/>
+    <hyperlink ref="B104" r:id="rId4" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0DBF3B46-CE41-6F47-A9AB-9D7CD028C4D7}"/>
+    <hyperlink ref="A103" r:id="rId5" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9C89488A-0EC9-394D-B0A4-D64F935C81B5}"/>
+    <hyperlink ref="B103" r:id="rId6" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{792FD4A7-487B-2C40-BFE1-AEC42FBFB293}"/>
+    <hyperlink ref="A29" r:id="rId7" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{90D6B942-0E98-D241-BD26-95CE598DF3B9}"/>
+    <hyperlink ref="B29" r:id="rId8" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8BE7B4F9-1DF9-F04E-AC92-6CA4F62CD203}"/>
+    <hyperlink ref="A76" r:id="rId9" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E6D0E3F7-CD58-FD4C-9E39-C24DD79A9F6E}"/>
+    <hyperlink ref="B76" r:id="rId10" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C5F9FE61-55B2-A246-8F3B-3A3B8661D501}"/>
+    <hyperlink ref="A49" r:id="rId11" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E7466E9F-D019-0148-B801-156422775032}"/>
+    <hyperlink ref="B49" r:id="rId12" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2A37D300-9C54-B24C-B371-3B394F1720C2}"/>
+    <hyperlink ref="A4" r:id="rId13" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FAC8E74B-DABF-5A44-92EF-1E29D7E2AE33}"/>
+    <hyperlink ref="B4" r:id="rId14" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AC0DCE32-B021-FA49-88F8-6B4551ED1E9B}"/>
+    <hyperlink ref="A105" r:id="rId15" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E6753A84-3826-6C4B-8E31-5883A166248A}"/>
+    <hyperlink ref="B105" r:id="rId16" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7F9FE7FC-DD40-8E4D-AE38-056EEF6C4B6A}"/>
+    <hyperlink ref="A30" r:id="rId17" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{60E7F68C-7892-2546-9D7E-57973E184572}"/>
+    <hyperlink ref="B30" r:id="rId18" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4DD56BA5-5525-AA48-8554-6773DFD615E1}"/>
+    <hyperlink ref="A5" r:id="rId19" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D8311BEF-9A52-2E49-9B1C-A7E5CE35523F}"/>
+    <hyperlink ref="B5" r:id="rId20" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{91725891-558E-B040-88F7-5FD3E71BD3D4}"/>
+    <hyperlink ref="A77" r:id="rId21" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3105DD9E-9800-5247-83AB-6265C3E48283}"/>
+    <hyperlink ref="B77" r:id="rId22" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D39879F8-416C-A84C-9CB6-8982FC0A851C}"/>
+    <hyperlink ref="A50" r:id="rId23" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3ABAF7A1-5B15-3F46-8ECD-C26AE6D80EEC}"/>
+    <hyperlink ref="B50" r:id="rId24" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AE9C9194-35D2-1745-AD18-2BAA06F465D9}"/>
+    <hyperlink ref="A106" r:id="rId25" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BB95714E-1CC6-9E4B-9E41-FB43B887FDB6}"/>
+    <hyperlink ref="B106" r:id="rId26" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{001BB2D5-579E-064E-8225-CCEA687C211B}"/>
+    <hyperlink ref="A31" r:id="rId27" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CA63A1EA-89EF-7640-B3FA-17E080AD2DB7}"/>
+    <hyperlink ref="B31" r:id="rId28" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{91F07258-3CFF-0548-A30D-7AE4FB392C7F}"/>
+    <hyperlink ref="A6" r:id="rId29" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5A6E0B15-C7F8-FE46-A1C6-163CB21ABF1E}"/>
+    <hyperlink ref="B6" r:id="rId30" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1A569BF5-093D-F444-AE93-EBD27047FF6C}"/>
+    <hyperlink ref="A78" r:id="rId31" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5EDC543F-E4CD-5140-A9EE-6715919C9243}"/>
+    <hyperlink ref="B78" r:id="rId32" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2FF83350-CFC8-514F-8616-688944A96481}"/>
+    <hyperlink ref="A51" r:id="rId33" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{60861CD7-53A1-6840-ADDC-3A269BAF3725}"/>
+    <hyperlink ref="B51" r:id="rId34" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{430444DB-450A-9041-9A56-A427A30AB50A}"/>
+    <hyperlink ref="A52" r:id="rId35" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{63742DCA-8957-3049-AE5F-D5EFB3670920}"/>
+    <hyperlink ref="B52" r:id="rId36" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C4D109D4-3C48-1244-AF8C-77C8EFE7BD26}"/>
+    <hyperlink ref="A79" r:id="rId37" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7CE1622F-1B13-DF45-86B6-472C6CB5D393}"/>
+    <hyperlink ref="B79" r:id="rId38" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{20A905E6-52F2-1E41-9ACF-44AE932405D0}"/>
+    <hyperlink ref="A7" r:id="rId39" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{648F0378-9C68-E044-8F64-AD8960E3C2F2}"/>
+    <hyperlink ref="B7" r:id="rId40" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B1805545-0A02-1E4E-94A3-28CB50BB3187}"/>
+    <hyperlink ref="A32" r:id="rId41" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{450273D2-0512-E945-B516-D151545EDE96}"/>
+    <hyperlink ref="B32" r:id="rId42" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A1C7C0AD-0FF8-294F-8DC6-E1C44591B123}"/>
+    <hyperlink ref="A114" r:id="rId43" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D74FFFFA-2A19-ED43-A761-261E77E428D4}"/>
+    <hyperlink ref="B114" r:id="rId44" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4855B6EE-367A-F14C-A83D-26C21191431D}"/>
+    <hyperlink ref="A33" r:id="rId45" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2DCD7E43-E147-6944-B52F-4B2CC63943FD}"/>
+    <hyperlink ref="B33" r:id="rId46" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8BC2FC7A-1806-F542-8062-1DE19A94EE57}"/>
+    <hyperlink ref="A8" r:id="rId47" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CAA15136-7CAB-AA41-A0C4-954658650ED7}"/>
+    <hyperlink ref="B8" r:id="rId48" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{42F2AFE5-4B42-7147-A5FC-8A06B02E69D1}"/>
+    <hyperlink ref="A53" r:id="rId49" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{511BDFD4-A1A3-9D4B-8EE1-84A16FEA9061}"/>
+    <hyperlink ref="B53" r:id="rId50" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8956FEDD-D077-A743-97E6-45801CF0010C}"/>
+    <hyperlink ref="A80" r:id="rId51" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E1F7D9A1-8477-2942-908C-1417F2810CD3}"/>
+    <hyperlink ref="B80" r:id="rId52" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F5387F0E-E426-0446-B9E5-04A856A47F2C}"/>
+    <hyperlink ref="A115" r:id="rId53" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{DA39E28B-52ED-8949-AD7B-5EDF3B64411B}"/>
+    <hyperlink ref="B115" r:id="rId54" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{685D6594-1E9C-DC44-9D8F-52CDB936B1C3}"/>
+    <hyperlink ref="A34" r:id="rId55" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6D142DAA-99C4-A140-A9D2-7C1F5C05641B}"/>
+    <hyperlink ref="B34" r:id="rId56" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A990774D-4F96-7441-A4D3-D6D4437BFF69}"/>
+    <hyperlink ref="A9" r:id="rId57" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{98574327-6BAF-2640-B82C-82111E4849B7}"/>
+    <hyperlink ref="B9" r:id="rId58" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AB768C97-E8D5-6948-886C-5BC8C8ED1F73}"/>
+    <hyperlink ref="A54" r:id="rId59" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E0F990EB-F729-7042-B024-01AE6A83AB8C}"/>
+    <hyperlink ref="B54" r:id="rId60" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4F718C52-3A54-D641-9E05-73026DE862BB}"/>
+    <hyperlink ref="A81" r:id="rId61" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0932E18C-0B9D-724C-9DE7-4688330A8B59}"/>
+    <hyperlink ref="B81" r:id="rId62" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BD05231F-4288-9B43-B737-5538F32D4408}"/>
+    <hyperlink ref="A116" r:id="rId63" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D7ED2EF8-EB33-4245-A23A-2E36EE4AE5A5}"/>
+    <hyperlink ref="B116" r:id="rId64" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{222CDD13-D029-C94B-8FFA-A640143F6494}"/>
+    <hyperlink ref="A35" r:id="rId65" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{19C29BA3-FF80-014B-8D6D-C932313E5465}"/>
+    <hyperlink ref="B35" r:id="rId66" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{01B37D6B-ED3A-0A48-BCA2-A05914065432}"/>
+    <hyperlink ref="A10" r:id="rId67" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1858DE3D-46DE-DB40-AB0C-D5422FDC8545}"/>
+    <hyperlink ref="B10" r:id="rId68" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3ECCE080-9470-A74D-8C59-108B508C18D2}"/>
+    <hyperlink ref="A55" r:id="rId69" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{82DB3069-AF5B-3C43-89B3-7C0C284F8280}"/>
+    <hyperlink ref="B55" r:id="rId70" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{77F23039-ADB1-4747-A298-4B9A26F18C6A}"/>
+    <hyperlink ref="A82" r:id="rId71" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0889E09F-2CBB-B047-9B10-EF1779FC78C9}"/>
+    <hyperlink ref="B82" r:id="rId72" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{11601384-370E-9F4E-9308-92C5B41E6523}"/>
+    <hyperlink ref="A117" r:id="rId73" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{85E5BAF5-E49E-4943-B16D-200F5A36DB51}"/>
+    <hyperlink ref="B117" r:id="rId74" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0ECE5547-A28A-E947-8177-2B454E160EAB}"/>
+    <hyperlink ref="A36" r:id="rId75" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{035BFBEC-CF08-CC45-B4B1-AA07A9B652F1}"/>
+    <hyperlink ref="B36" r:id="rId76" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{81F8EDB6-4D97-244C-9EC6-1C7015A1C3AA}"/>
+    <hyperlink ref="A11" r:id="rId77" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B667DA40-CB68-8D4B-9F4B-754B464A81EF}"/>
+    <hyperlink ref="B11" r:id="rId78" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C9A26BBB-3DFD-CD4C-9D68-2F66D5B16845}"/>
+    <hyperlink ref="A56" r:id="rId79" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D3F4F7EC-0D20-634E-BC18-501A43C0FF20}"/>
+    <hyperlink ref="B56" r:id="rId80" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{14A57ABC-A865-E149-ABC7-5B2FA0703CF4}"/>
+    <hyperlink ref="A83" r:id="rId81" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F596C5CE-7549-5745-8C01-E13C2E6C3EDD}"/>
+    <hyperlink ref="B83" r:id="rId82" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B4CB320E-E905-7D4D-B75C-E9C029A9D8A5}"/>
+    <hyperlink ref="A118" r:id="rId83" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3063A68B-3AE8-2442-A649-C1249A24A103}"/>
+    <hyperlink ref="B118" r:id="rId84" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AE9A451D-8D82-EC4D-9E6F-5943BFB8217C}"/>
+    <hyperlink ref="A37" r:id="rId85" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9B480080-893E-094B-9D79-5AAAE31E4FF9}"/>
+    <hyperlink ref="B37" r:id="rId86" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D85CA6A9-03E0-EB42-8CBD-806F9396F890}"/>
+    <hyperlink ref="A12" r:id="rId87" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BF14926D-3505-0D47-AECB-28361A0F9849}"/>
+    <hyperlink ref="B12" r:id="rId88" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{DE3477C6-B6B7-044C-A8EC-E361E6DEC490}"/>
+    <hyperlink ref="A57" r:id="rId89" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F495A9F5-FF48-094F-8023-FCB478B64F8B}"/>
+    <hyperlink ref="B57" r:id="rId90" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E09B6D4F-374F-7B40-9D95-3D1A2832E13C}"/>
+    <hyperlink ref="A84" r:id="rId91" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A285C9EC-7A57-B442-8B71-71BE7715A4B8}"/>
+    <hyperlink ref="B84" r:id="rId92" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C47D91C1-A113-0A48-84FA-241E27D8A834}"/>
+    <hyperlink ref="A119" r:id="rId93" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CE263224-1AE0-3F4B-B195-161EDBB2AFBC}"/>
+    <hyperlink ref="B119" r:id="rId94" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{82B5B924-7646-FD42-8C0D-C1BA8A4DBE77}"/>
+    <hyperlink ref="A38" r:id="rId95" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6BB1B06F-4302-D24C-9AC3-A4FD81D49E3B}"/>
+    <hyperlink ref="B38" r:id="rId96" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{93994046-9E22-344C-ABDE-580E9E60486F}"/>
+    <hyperlink ref="A13" r:id="rId97" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{521130E2-22F7-474F-B6B9-AD81A07D3AA9}"/>
+    <hyperlink ref="B13" r:id="rId98" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F2D4F1C8-8C7F-3A4D-A5F8-609AC98AC07C}"/>
+    <hyperlink ref="A58" r:id="rId99" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E09F3732-ECB0-F04A-A61D-A51F243A5A06}"/>
+    <hyperlink ref="B58" r:id="rId100" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{17E83ABE-664D-E742-BCBE-3892F42B759D}"/>
+    <hyperlink ref="A85" r:id="rId101" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A99708A7-CA03-1D41-ADA2-BE0805AC9D75}"/>
+    <hyperlink ref="B85" r:id="rId102" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3AD8F48A-98AF-6F49-8A7A-09784D3398C4}"/>
+    <hyperlink ref="A120" r:id="rId103" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BC09DCE5-F265-3A46-B790-E839FC9EDF50}"/>
+    <hyperlink ref="B120" r:id="rId104" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{17F2CD0C-CF11-DC4A-A55B-9ED6155B8966}"/>
+    <hyperlink ref="A39" r:id="rId105" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A9BC2794-01FC-A846-A286-8BF225161508}"/>
+    <hyperlink ref="B39" r:id="rId106" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3C781BDC-DFDC-B649-A43C-1821BACDB164}"/>
+    <hyperlink ref="A14" r:id="rId107" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5D4B418A-DC15-1C47-9A6F-033914E544AE}"/>
+    <hyperlink ref="B14" r:id="rId108" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{DF5E125A-DB5F-B347-9678-E184CAF4534E}"/>
+    <hyperlink ref="A59" r:id="rId109" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6B2399E3-5E0B-1844-BD69-A79BD447731E}"/>
+    <hyperlink ref="B59" r:id="rId110" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{58F5442A-6E36-6844-87A6-B951185FFDF8}"/>
+    <hyperlink ref="A86" r:id="rId111" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F0BB8FFE-1E40-7D41-BEB0-8924A425CBF6}"/>
+    <hyperlink ref="B86" r:id="rId112" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8F5B32FC-3D92-3A47-A1C1-D7B54C9E2C7D}"/>
+    <hyperlink ref="A121" r:id="rId113" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5B0AAC23-1E90-C34A-B49C-BED91C8FEB9B}"/>
+    <hyperlink ref="B121" r:id="rId114" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8A66EA9C-2D29-2E4C-9711-FD3A9A906649}"/>
+    <hyperlink ref="A40" r:id="rId115" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{35EF7048-B226-AE4B-9A6F-EB88AA52C4D2}"/>
+    <hyperlink ref="B40" r:id="rId116" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E1C44D48-EE93-7240-9ECF-F4E61B0555B8}"/>
+    <hyperlink ref="A15" r:id="rId117" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{00426CFB-D028-7F4D-8208-34F1960BE322}"/>
+    <hyperlink ref="B15" r:id="rId118" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9E018437-9DD8-D34F-8AC5-B20AB0BBA577}"/>
+    <hyperlink ref="A60" r:id="rId119" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FBA64D05-E6D7-654C-9464-A139D737FC01}"/>
+    <hyperlink ref="B60" r:id="rId120" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{054EFC24-F385-DA40-96B5-5C1A37E87AE9}"/>
+    <hyperlink ref="A87" r:id="rId121" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{291BB87D-15E7-3546-A607-84D80B6BE82C}"/>
+    <hyperlink ref="B87" r:id="rId122" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B1F99796-1718-9E48-A0E8-52BA090EE93D}"/>
+    <hyperlink ref="A122" r:id="rId123" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1BA59FFC-5B07-6244-AD29-EA835AB3B99C}"/>
+    <hyperlink ref="B122" r:id="rId124" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CF2B51EF-5F4A-D94C-85F6-34CC8D1BDAB0}"/>
+    <hyperlink ref="A41" r:id="rId125" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{99F7F470-316F-5746-AD42-6CC5CA4AC540}"/>
+    <hyperlink ref="B41" r:id="rId126" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{232A06FD-399A-0244-8507-8B13B5D229EA}"/>
+    <hyperlink ref="A16" r:id="rId127" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D0562D2F-0779-A240-9F76-9ED48E9EF76A}"/>
+    <hyperlink ref="B16" r:id="rId128" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{583E2B2A-5DC5-A44E-9DB2-3D98CDA5D6F6}"/>
+    <hyperlink ref="A61" r:id="rId129" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A0AEC1A8-DF56-284E-A673-618B7F2E8D3E}"/>
+    <hyperlink ref="B61" r:id="rId130" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B0F94F40-B346-1843-BA29-4D068B2B8666}"/>
+    <hyperlink ref="A88" r:id="rId131" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5F643EE0-7739-C84B-9DCA-BDB2EFFF65AE}"/>
+    <hyperlink ref="B88" r:id="rId132" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BC7B17FA-DDA9-A84F-A40A-D8D9CDB7B2C0}"/>
+    <hyperlink ref="A123" r:id="rId133" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FABD9A06-2A56-CE49-A44B-42AD8524CBFE}"/>
+    <hyperlink ref="B123" r:id="rId134" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CB65410B-9662-FC45-A425-16BA7941AECE}"/>
+    <hyperlink ref="A42" r:id="rId135" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FE326F2B-AE00-AE4C-8883-B546235B28E8}"/>
+    <hyperlink ref="B42" r:id="rId136" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4E5337A8-81EB-314B-AF8F-90D4EB44C3C2}"/>
+    <hyperlink ref="A17" r:id="rId137" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{701D7B8F-1AB1-F548-91EB-4E02FF574414}"/>
+    <hyperlink ref="B17" r:id="rId138" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B2592F3B-3F1E-7945-B04C-1AFADA87D37A}"/>
+    <hyperlink ref="A62" r:id="rId139" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2F23F754-CDDC-514A-B309-E008DF0955AD}"/>
+    <hyperlink ref="B62" r:id="rId140" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BC9F9EA4-7699-A74D-9179-AA990230D20F}"/>
+    <hyperlink ref="A89" r:id="rId141" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{801A81C8-4B95-7343-A8FC-D97F1B9AB629}"/>
+    <hyperlink ref="B89" r:id="rId142" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0EFF83A4-08A7-E343-8DFC-C63E9E1700F0}"/>
+    <hyperlink ref="A130" r:id="rId143" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{97E36A89-0E63-6F43-BDAE-600FAECDAF2C}"/>
+    <hyperlink ref="B130" r:id="rId144" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{501069B2-1236-964D-BA4E-EED81AA8F971}"/>
+    <hyperlink ref="A43" r:id="rId145" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{25B09CC3-BE6C-7345-98C6-C195C451FDB7}"/>
+    <hyperlink ref="B43" r:id="rId146" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D16EC1B0-ACF6-3141-B15F-C204E105D399}"/>
+    <hyperlink ref="A18" r:id="rId147" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3E271FFD-2F50-3B4D-868F-6E6C8868937F}"/>
+    <hyperlink ref="B18" r:id="rId148" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E3782E41-433A-434B-8FA1-5C1DF82F22D6}"/>
+    <hyperlink ref="A63" r:id="rId149" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{822F21CB-3B91-C94A-A69C-851E258B3504}"/>
+    <hyperlink ref="B63" r:id="rId150" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{00897AAC-66BA-E149-9E30-BA440A0855B5}"/>
+    <hyperlink ref="A90" r:id="rId151" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3730C8B6-974D-E946-9EB0-A863F083F0B4}"/>
+    <hyperlink ref="B90" r:id="rId152" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C7700CC3-1F37-9243-B9FF-C3439553A2FF}"/>
+    <hyperlink ref="A124" r:id="rId153" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{34192A77-883A-7C47-838D-4FFA58C1858F}"/>
+    <hyperlink ref="B124" r:id="rId154" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{69712FA0-C681-964D-8964-11B2B5EBE224}"/>
+    <hyperlink ref="A44" r:id="rId155" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A400B5A0-A940-5C40-A9C9-610F9D8595F4}"/>
+    <hyperlink ref="B44" r:id="rId156" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FD8D029E-8D4C-3449-A185-0553FB6058E6}"/>
+    <hyperlink ref="A19" r:id="rId157" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9D98353B-D99E-064B-9939-0C4BE350252D}"/>
+    <hyperlink ref="B19" r:id="rId158" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6175D7C5-9E51-B948-A28C-652E73B0BAD1}"/>
+    <hyperlink ref="A64" r:id="rId159" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{27361F2B-A345-1646-AF3A-8520D2BFDD73}"/>
+    <hyperlink ref="B64" r:id="rId160" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BC4171C1-83B1-6F44-97B3-C5E94F629FE9}"/>
+    <hyperlink ref="A91" r:id="rId161" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{56AF9B9C-6206-8149-97AF-5D51FF84F1E0}"/>
+    <hyperlink ref="B91" r:id="rId162" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7D6FD9A3-F472-FF45-AF14-F5A702C3B574}"/>
+    <hyperlink ref="A45" r:id="rId163" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F9C41EE9-C6F1-A248-BC92-A9EEEE29B69B}"/>
+    <hyperlink ref="B45" r:id="rId164" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3A799C30-7E46-5345-9CD9-5A00D2D8FCB6}"/>
+    <hyperlink ref="A20" r:id="rId165" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{45E3CEA5-41DB-2D48-9DC6-A37CC10FE398}"/>
+    <hyperlink ref="B20" r:id="rId166" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{78B7063F-DD6A-D344-862B-CCF6791FBB71}"/>
+    <hyperlink ref="A65" r:id="rId167" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4935C5D5-059E-CB41-A043-D2AE4ABB8EED}"/>
+    <hyperlink ref="B65" r:id="rId168" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{175AC589-D93C-204C-AE6A-FEB6E52B843E}"/>
+    <hyperlink ref="A92" r:id="rId169" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{70AB2F48-545E-F247-A698-9AFF74761AA6}"/>
+    <hyperlink ref="B92" r:id="rId170" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BBAACB40-4602-5443-BCC5-5D3C6DF4A126}"/>
+    <hyperlink ref="A125" r:id="rId171" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{323F460F-FFA9-3644-BB41-BFFC20F524AF}"/>
+    <hyperlink ref="B125" r:id="rId172" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{55631538-3829-B743-87D2-4356C058BAAC}"/>
+    <hyperlink ref="A126" r:id="rId173" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FE1CCEA8-77EE-8943-8E7F-96C66AAB5410}"/>
+    <hyperlink ref="B126" r:id="rId174" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E6995AB4-8050-5D40-8EC3-368BCA76B6BF}"/>
+    <hyperlink ref="A46" r:id="rId175" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AAEEBDC0-5171-4C48-A5FC-15673B47806F}"/>
+    <hyperlink ref="B46" r:id="rId176" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{BC4F41DF-E001-8D40-A7FF-8B6B4058DFF9}"/>
+    <hyperlink ref="A21" r:id="rId177" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{49ADC0F9-C948-A24D-86D8-916A69DC3584}"/>
+    <hyperlink ref="B21" r:id="rId178" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{A5C9F8C4-9E95-7A44-8798-21F8B542F02D}"/>
+    <hyperlink ref="A66" r:id="rId179" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B5FE8245-6634-654E-946F-24F1891A5964}"/>
+    <hyperlink ref="B66" r:id="rId180" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D0708BE2-D2ED-2547-A7CE-AB87D5C8C314}"/>
+    <hyperlink ref="A93" r:id="rId181" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{97EDCEAA-D7BF-EA49-8C48-57DE32207AEF}"/>
+    <hyperlink ref="B93" r:id="rId182" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{39D0380A-E06E-434B-A765-81B21CF8502E}"/>
+    <hyperlink ref="A127" r:id="rId183" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2A9EFA11-147E-BB47-9A51-AEF03BA914D6}"/>
+    <hyperlink ref="B127" r:id="rId184" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{37B31F2A-AD32-8F4F-AE44-CC499C4A2453}"/>
+    <hyperlink ref="A22" r:id="rId185" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C637B83D-0BAC-E043-954A-37EA7C80473D}"/>
+    <hyperlink ref="B22" r:id="rId186" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B33FD101-C6B2-9F4B-8B99-392AC091FABF}"/>
+    <hyperlink ref="A67" r:id="rId187" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{77AD125E-73EB-404E-924A-722B5EAC350D}"/>
+    <hyperlink ref="B67" r:id="rId188" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4F9B76ED-8112-A34C-81A1-6885E5D9CBC1}"/>
+    <hyperlink ref="A94" r:id="rId189" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7775DAC5-884C-C146-9048-17D2A47AAB40}"/>
+    <hyperlink ref="B94" r:id="rId190" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{F377990E-202F-5242-9287-69FA74587CD0}"/>
+    <hyperlink ref="A107" r:id="rId191" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8B0167F1-7685-2F48-BA4C-7EE8190834B5}"/>
+    <hyperlink ref="B107" r:id="rId192" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B31680E4-3115-6C44-A118-ABD7938D5415}"/>
+    <hyperlink ref="A23" r:id="rId193" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8A27F802-DD5D-6B43-8526-7D0F8B569E8F}"/>
+    <hyperlink ref="B23" r:id="rId194" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{382A0674-3C1F-BB4A-B763-9CA070B29F82}"/>
+    <hyperlink ref="A68" r:id="rId195" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{41E1FB60-2009-8B49-AD94-5D160D40360A}"/>
+    <hyperlink ref="B68" r:id="rId196" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{66B27388-5C34-D24D-9156-8E3E884D4FAD}"/>
+    <hyperlink ref="A95" r:id="rId197" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{525B215A-6626-7C4A-8428-9564EA714C7D}"/>
+    <hyperlink ref="B95" r:id="rId198" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{EE679002-B9DC-C745-9F96-171B41CDF9BD}"/>
+    <hyperlink ref="A108" r:id="rId199" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{17F7F569-26F6-D649-A334-0876D7177BCA}"/>
+    <hyperlink ref="B108" r:id="rId200" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B83E2A32-D0F5-8B42-BE5A-15691AB2FC36}"/>
+    <hyperlink ref="A24" r:id="rId201" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{58AFB1D5-9D4D-C64A-8D34-1BD9FA22C9A6}"/>
+    <hyperlink ref="B24" r:id="rId202" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{926B7348-A4C6-4E46-81A9-4BE2CA65F3A3}"/>
+    <hyperlink ref="A69" r:id="rId203" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{ADE53C0B-02AE-FE41-BCE5-D156CADE871E}"/>
+    <hyperlink ref="B69" r:id="rId204" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{8EA69992-9344-AA41-9A7A-5FFC8855DEBD}"/>
+    <hyperlink ref="A96" r:id="rId205" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{96CE9CB9-E37E-C249-85DD-5C74B3DE328D}"/>
+    <hyperlink ref="B96" r:id="rId206" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9176854D-3207-2548-98EE-FEAE859C6517}"/>
+    <hyperlink ref="A109" r:id="rId207" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{AD1F066A-6289-9044-9E54-DFE9A907B25A}"/>
+    <hyperlink ref="B109" r:id="rId208" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{0C90B533-485B-C14C-A900-7870F8A70280}"/>
+    <hyperlink ref="A47" r:id="rId209" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2D2B7CF6-9B8A-6C4C-8DB1-94C987B1DA59}"/>
+    <hyperlink ref="B47" r:id="rId210" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9469212A-DE6B-674D-AB49-6A93AF6A670E}"/>
+    <hyperlink ref="A25" r:id="rId211" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{50360F3E-9DF6-7E46-AD1A-390EACEC8895}"/>
+    <hyperlink ref="B25" r:id="rId212" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{E6CB33C1-BE7C-FF4E-A133-D14C4599BF4B}"/>
+    <hyperlink ref="A70" r:id="rId213" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B06D0835-2F6D-7844-A9FC-549129BD6323}"/>
+    <hyperlink ref="B70" r:id="rId214" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CD9E5FFF-91C5-C34D-B89E-EF15A3A64F4E}"/>
+    <hyperlink ref="A97" r:id="rId215" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6B77A06B-3F5C-3040-B7BB-1FE657DFD7B6}"/>
+    <hyperlink ref="B97" r:id="rId216" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{CC1EC814-7DFB-F245-9952-6C52B8D40CC2}"/>
+    <hyperlink ref="A128" r:id="rId217" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{93FCCC25-8671-9D4B-A3DD-482BB79D7759}"/>
+    <hyperlink ref="B128" r:id="rId218" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3F2CC9E0-958C-BF45-9773-8BE446FE5D41}"/>
+    <hyperlink ref="A26" r:id="rId219" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{02A02B34-0D47-D04A-8F9F-36F1A8FEE537}"/>
+    <hyperlink ref="B26" r:id="rId220" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{ADDEEE70-213E-7445-BC80-E18D4D5CD8D2}"/>
+    <hyperlink ref="A71" r:id="rId221" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7ECCDEE0-23FD-0247-AEE9-728F49253E15}"/>
+    <hyperlink ref="B71" r:id="rId222" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{04BC4D55-D4BF-9F45-ABA8-B2108CC5DFE6}"/>
+    <hyperlink ref="A98" r:id="rId223" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{C749C834-77A6-8345-A28C-AC5D12879DC0}"/>
+    <hyperlink ref="B98" r:id="rId224" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{EDB26659-0767-BB47-BF7D-1E35933A94E2}"/>
+    <hyperlink ref="A129" r:id="rId225" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D59CDA39-267A-A841-B4DA-EF61AEB02F87}"/>
+    <hyperlink ref="B129" r:id="rId226" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{174F795C-A5D9-EF4D-9547-9FFE60C45AC8}"/>
+    <hyperlink ref="A27" r:id="rId227" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1EC43E3E-035E-EB40-BDB2-0391B5A3518D}"/>
+    <hyperlink ref="B27" r:id="rId228" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{352F687D-512E-8045-BEE1-1EB3F005F259}"/>
+    <hyperlink ref="A72" r:id="rId229" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{B06D7473-A1CA-FD4D-9B09-D2B8543D88DB}"/>
+    <hyperlink ref="B72" r:id="rId230" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{4FB6AEE3-950D-7144-AB63-81CD955B592D}"/>
+    <hyperlink ref="A99" r:id="rId231" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{58AE7BE0-A023-FE4D-ABCA-EB1CE235FBB7}"/>
+    <hyperlink ref="B99" r:id="rId232" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D731C2FE-9D39-1041-80DA-B4E880F97491}"/>
+    <hyperlink ref="A110" r:id="rId233" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D901ECF2-897B-A44C-B4D7-07D2BFDF5447}"/>
+    <hyperlink ref="B110" r:id="rId234" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{08131EB6-6170-AA4A-9481-B821264CCEA3}"/>
+    <hyperlink ref="A28" r:id="rId235" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{82DD1044-8A35-9E4E-97B2-078F79AAF36B}"/>
+    <hyperlink ref="B28" r:id="rId236" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{195DCC4F-C3CA-4244-A2F7-4D59361F10C9}"/>
+    <hyperlink ref="A73" r:id="rId237" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1D1759E1-AF5C-5840-AC8B-E4D42AED4E31}"/>
+    <hyperlink ref="B73" r:id="rId238" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{DA6AC16B-FDEC-AA40-8793-7B47E617B435}"/>
+    <hyperlink ref="A100" r:id="rId239" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{6AE1501F-6764-9944-89FE-0F2F3DF5A864}"/>
+    <hyperlink ref="B100" r:id="rId240" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{09A667F1-FA76-7A44-8F8C-31E0F9BD84FA}"/>
+    <hyperlink ref="A111" r:id="rId241" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{92288B91-1C89-2446-91B5-B1567D93A6D8}"/>
+    <hyperlink ref="B111" r:id="rId242" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{2D57E4D7-9DAD-BE4F-975D-3227E12D3937}"/>
+    <hyperlink ref="A2" r:id="rId243" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{DF895207-E102-0C4F-95A2-21A3D1473448}"/>
+    <hyperlink ref="B2" r:id="rId244" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{484923DE-E31F-8247-B020-ACC0EF01C322}"/>
+    <hyperlink ref="A74" r:id="rId245" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{82BB7F3F-9518-4943-816A-605FD06C43F1}"/>
+    <hyperlink ref="B74" r:id="rId246" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{7362E52C-523D-A844-9022-11FE65CA51F0}"/>
+    <hyperlink ref="A101" r:id="rId247" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{72CC6A1B-FEEE-0A4D-816D-3ED047FD5D79}"/>
+    <hyperlink ref="B101" r:id="rId248" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{EC967DE3-2C47-744B-B151-A6F90AC841F6}"/>
+    <hyperlink ref="A112" r:id="rId249" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{84FA3D3A-B3E7-E844-891B-F944399E1886}"/>
+    <hyperlink ref="B112" r:id="rId250" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{1DED175B-A3AF-4F4B-8382-7E6797F7C9A5}"/>
+    <hyperlink ref="A3" r:id="rId251" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5BF7F73E-C528-4E47-9882-2EF68AB470AA}"/>
+    <hyperlink ref="B3" r:id="rId252" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{29DC4BCD-6CB7-5F49-98EF-8A857F83C23B}"/>
+    <hyperlink ref="A75" r:id="rId253" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{9B351D1D-9311-8A4E-8A99-95F6A55EAD09}"/>
+    <hyperlink ref="B75" r:id="rId254" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{FC3B5D8B-97B8-C140-801E-E6D4279DAC83}"/>
+    <hyperlink ref="A102" r:id="rId255" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{83C0EB1A-102B-214C-8E4E-B5B7392AE84F}"/>
+    <hyperlink ref="B102" r:id="rId256" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{3B6729CA-7004-324F-B659-A636199078F2}"/>
+    <hyperlink ref="B113" r:id="rId257" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{D6821C3C-B8D3-6043-8B13-35BA2219EAF9}"/>
+    <hyperlink ref="A113" r:id="rId258" display="https://www.nlsinfo.org/investigator/pages/search?s=NLSY79" xr:uid="{5F2C9A09-38B4-9848-AA52-E45D955CBEF2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Made some small changes and added summary statistics.
</commit_message>
<xml_diff>
--- a/src/original_data/var_info.xlsx
+++ b/src/original_data/var_info.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berfinbinzet/Desktop/EPP_Project/project/Final_Project/original_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/berfinbinzet/Desktop/EPP_Project/project/Final_Project/src/original_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A7983EB-41D7-B24C-8543-146D875FF56D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04305E4B-12FD-B44C-AFDF-9EC1EF85B783}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="600" windowWidth="26340" windowHeight="14080" xr2:uid="{3D1ABEF0-DFAA-F34E-8AFF-D9F108717ACA}"/>
   </bookViews>
@@ -474,9 +474,6 @@
     <t>sex</t>
   </si>
   <si>
-    <t>employment_status</t>
-  </si>
-  <si>
     <t>weeks_worked</t>
   </si>
   <si>
@@ -487,6 +484,9 @@
   </si>
   <si>
     <t>invariant</t>
+  </si>
+  <si>
+    <t>participation</t>
   </si>
 </sst>
 </file>
@@ -858,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A88ECB0D-008C-0041-B40C-8251D6DFE406}">
   <dimension ref="A1:D130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -889,7 +889,7 @@
         <v>87</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D2" s="1">
         <v>2014</v>
@@ -903,7 +903,7 @@
         <v>87</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D3" s="1">
         <v>2016</v>
@@ -917,7 +917,7 @@
         <v>87</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D4" s="1">
         <v>1979</v>
@@ -931,7 +931,7 @@
         <v>87</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D5" s="1">
         <v>1980</v>
@@ -945,7 +945,7 @@
         <v>87</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D6" s="1">
         <v>1981</v>
@@ -959,7 +959,7 @@
         <v>87</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D7" s="1">
         <v>1982</v>
@@ -973,7 +973,7 @@
         <v>87</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" s="1">
         <v>1983</v>
@@ -987,7 +987,7 @@
         <v>87</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D9" s="1">
         <v>1984</v>
@@ -1001,7 +1001,7 @@
         <v>87</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D10" s="1">
         <v>1985</v>
@@ -1015,7 +1015,7 @@
         <v>87</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D11" s="1">
         <v>1986</v>
@@ -1029,7 +1029,7 @@
         <v>87</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D12" s="1">
         <v>1987</v>
@@ -1043,7 +1043,7 @@
         <v>87</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D13" s="1">
         <v>1988</v>
@@ -1057,7 +1057,7 @@
         <v>87</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D14" s="1">
         <v>1989</v>
@@ -1071,7 +1071,7 @@
         <v>87</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D15" s="1">
         <v>1990</v>
@@ -1085,7 +1085,7 @@
         <v>87</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D16" s="1">
         <v>1991</v>
@@ -1099,7 +1099,7 @@
         <v>87</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D17" s="1">
         <v>1992</v>
@@ -1113,7 +1113,7 @@
         <v>87</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D18" s="1">
         <v>1993</v>
@@ -1127,7 +1127,7 @@
         <v>87</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D19" s="1">
         <v>1994</v>
@@ -1141,7 +1141,7 @@
         <v>87</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D20" s="1">
         <v>1996</v>
@@ -1155,7 +1155,7 @@
         <v>87</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D21" s="1">
         <v>1998</v>
@@ -1169,7 +1169,7 @@
         <v>87</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D22" s="1">
         <v>2000</v>
@@ -1183,7 +1183,7 @@
         <v>87</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D23" s="1">
         <v>2002</v>
@@ -1197,7 +1197,7 @@
         <v>87</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D24" s="1">
         <v>2004</v>
@@ -1211,7 +1211,7 @@
         <v>87</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D25" s="1">
         <v>2006</v>
@@ -1225,7 +1225,7 @@
         <v>87</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D26" s="1">
         <v>2008</v>
@@ -1239,7 +1239,7 @@
         <v>87</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D27" s="1">
         <v>2010</v>
@@ -1253,7 +1253,7 @@
         <v>87</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D28" s="1">
         <v>2012</v>
@@ -1267,7 +1267,7 @@
         <v>57</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D29" s="1">
         <v>1979</v>
@@ -1281,7 +1281,7 @@
         <v>57</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D30" s="1">
         <v>1980</v>
@@ -1295,7 +1295,7 @@
         <v>57</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D31" s="1">
         <v>1981</v>
@@ -1309,7 +1309,7 @@
         <v>57</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D32" s="1">
         <v>1982</v>
@@ -1323,7 +1323,7 @@
         <v>57</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D33" s="1">
         <v>1983</v>
@@ -1337,7 +1337,7 @@
         <v>57</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D34" s="1">
         <v>1984</v>
@@ -1351,7 +1351,7 @@
         <v>57</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D35" s="1">
         <v>1985</v>
@@ -1365,7 +1365,7 @@
         <v>57</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D36" s="1">
         <v>1986</v>
@@ -1379,7 +1379,7 @@
         <v>57</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D37" s="1">
         <v>1987</v>
@@ -1393,7 +1393,7 @@
         <v>57</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D38" s="1">
         <v>1988</v>
@@ -1407,7 +1407,7 @@
         <v>57</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D39" s="1">
         <v>1989</v>
@@ -1421,7 +1421,7 @@
         <v>57</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D40" s="1">
         <v>1990</v>
@@ -1435,7 +1435,7 @@
         <v>57</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D41" s="1">
         <v>1991</v>
@@ -1449,7 +1449,7 @@
         <v>57</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D42" s="1">
         <v>1992</v>
@@ -1463,7 +1463,7 @@
         <v>57</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D43" s="1">
         <v>1993</v>
@@ -1477,7 +1477,7 @@
         <v>57</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D44" s="1">
         <v>1994</v>
@@ -1491,7 +1491,7 @@
         <v>57</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D45" s="1">
         <v>1996</v>
@@ -1505,7 +1505,7 @@
         <v>57</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D46" s="1">
         <v>1998</v>
@@ -1519,7 +1519,7 @@
         <v>57</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
       <c r="D47" s="1">
         <v>2006</v>
@@ -1533,10 +1533,10 @@
         <v>81</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="18" x14ac:dyDescent="0.2">
@@ -1925,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D76" s="1">
         <v>1978</v>
@@ -1939,7 +1939,7 @@
         <v>1</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D77" s="1">
         <v>1979</v>
@@ -1953,7 +1953,7 @@
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D78" s="1">
         <v>1980</v>
@@ -1967,7 +1967,7 @@
         <v>1</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D79" s="1">
         <v>1981</v>
@@ -1981,7 +1981,7 @@
         <v>1</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D80" s="1">
         <v>1982</v>
@@ -1995,7 +1995,7 @@
         <v>1</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D81" s="1">
         <v>1983</v>
@@ -2009,7 +2009,7 @@
         <v>1</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D82" s="1">
         <v>1984</v>
@@ -2023,7 +2023,7 @@
         <v>1</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D83" s="1">
         <v>1985</v>
@@ -2037,7 +2037,7 @@
         <v>1</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D84" s="1">
         <v>1986</v>
@@ -2051,7 +2051,7 @@
         <v>1</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D85" s="1">
         <v>1987</v>
@@ -2065,7 +2065,7 @@
         <v>1</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D86" s="1">
         <v>1988</v>
@@ -2079,7 +2079,7 @@
         <v>1</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D87" s="1">
         <v>1989</v>
@@ -2093,7 +2093,7 @@
         <v>1</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D88" s="1">
         <v>1990</v>
@@ -2107,7 +2107,7 @@
         <v>1</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D89" s="1">
         <v>1991</v>
@@ -2121,7 +2121,7 @@
         <v>1</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D90" s="1">
         <v>1992</v>
@@ -2135,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D91" s="1">
         <v>1993</v>
@@ -2149,7 +2149,7 @@
         <v>1</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D92" s="1">
         <v>1995</v>
@@ -2163,7 +2163,7 @@
         <v>1</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D93" s="1">
         <v>1997</v>
@@ -2177,7 +2177,7 @@
         <v>1</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D94" s="1">
         <v>1999</v>
@@ -2191,7 +2191,7 @@
         <v>1</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D95" s="1">
         <v>2001</v>
@@ -2205,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D96" s="1">
         <v>2003</v>
@@ -2219,7 +2219,7 @@
         <v>1</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D97" s="1">
         <v>2005</v>
@@ -2233,7 +2233,7 @@
         <v>1</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D98" s="1">
         <v>2007</v>
@@ -2247,7 +2247,7 @@
         <v>1</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D99" s="1">
         <v>2009</v>
@@ -2261,7 +2261,7 @@
         <v>1</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D100" s="1">
         <v>2011</v>
@@ -2275,7 +2275,7 @@
         <v>1</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D101" s="1">
         <v>2013</v>
@@ -2289,7 +2289,7 @@
         <v>1</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D102" s="1">
         <v>2015</v>
@@ -2306,7 +2306,7 @@
         <v>144</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="104" spans="1:4" ht="18" x14ac:dyDescent="0.2">

</xml_diff>